<commit_message>
languages changes code commit
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Osprey_EMEA/GoldOspreyemeaEUFR.xlsx
+++ b/src/test/resources/TestData/Osprey_EMEA/GoldOspreyemeaEUFR.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2F2AB01-8478-4F33-9C51-FD23DFB2330A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEA0F320-7CF6-40D2-8C1F-AEFEB71B84AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="9960" firstSheet="15" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="15" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1041" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1043" uniqueCount="292">
   <si>
     <t>UserName</t>
   </si>
@@ -925,6 +925,12 @@
   </si>
   <si>
     <t>€</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Sacs à dos et sacs</t>
+  </si>
+  <si>
+    <t>header</t>
   </si>
 </sst>
 </file>
@@ -3329,10 +3335,10 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DEDE721-2994-4A91-8C89-FADAE76105D8}">
-  <dimension ref="A1:AI29"/>
+  <dimension ref="A1:AJ29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3343,23 +3349,23 @@
     <col min="4" max="4" width="38" customWidth="1"/>
     <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="12.7109375" customWidth="1"/>
-    <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24" bestFit="1" customWidth="1"/>
-    <col min="12" max="15" width="12.7109375" customWidth="1"/>
-    <col min="16" max="17" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11" customWidth="1"/>
-    <col min="29" max="29" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="10" width="12.7109375" customWidth="1"/>
+    <col min="11" max="11" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24" bestFit="1" customWidth="1"/>
+    <col min="13" max="16" width="12.7109375" customWidth="1"/>
+    <col min="17" max="18" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11" customWidth="1"/>
+    <col min="30" max="30" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="23.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3379,94 +3385,97 @@
         <v>16</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>52</v>
       </c>
@@ -3494,117 +3503,118 @@
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
-      <c r="P2" t="s">
+      <c r="P2" s="2"/>
+      <c r="Q2" t="s">
         <v>48</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>98</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>285</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>286</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>287</v>
       </c>
-      <c r="U2" s="5">
+      <c r="V2" s="5">
         <v>36000</v>
       </c>
-      <c r="V2" s="5" t="s">
+      <c r="W2" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="W2" s="5"/>
-    </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="X2" s="5"/>
+    </row>
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>95</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="M3" s="5" t="s">
         <v>289</v>
       </c>
-      <c r="X3" t="s">
+      <c r="Y3" t="s">
         <v>257</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="Z3" t="s">
         <v>278</v>
       </c>
-      <c r="Z3" s="9" t="s">
+      <c r="AA3" s="9" t="s">
         <v>204</v>
       </c>
-      <c r="AA3" t="s">
+      <c r="AB3" t="s">
         <v>101</v>
       </c>
-      <c r="AB3" s="5" t="s">
+      <c r="AC3" s="5" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>100</v>
       </c>
-      <c r="AC4" t="s">
+      <c r="AD4" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>106</v>
       </c>
-      <c r="AD5" s="5" t="s">
+      <c r="AE5" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="AE5" s="7" t="s">
+      <c r="AF5" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="AF5">
+      <c r="AG5">
         <v>123</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>109</v>
       </c>
-      <c r="AD6" s="5" t="s">
+      <c r="AE6" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="AE6" s="7" t="s">
+      <c r="AF6" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="AF6">
+      <c r="AG6">
         <v>1234</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>111</v>
       </c>
-      <c r="AD7" s="5" t="s">
+      <c r="AE7" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="AE7" s="7" t="s">
+      <c r="AF7" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="AF7">
+      <c r="AG7">
         <v>123</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>113</v>
       </c>
-      <c r="AD8" s="5" t="s">
+      <c r="AE8" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="AE8" s="7" t="s">
+      <c r="AF8" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="AF8">
+      <c r="AG8">
         <v>123</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>46</v>
       </c>
@@ -3626,14 +3636,15 @@
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
-      <c r="P9" t="s">
+      <c r="P9" s="2"/>
+      <c r="Q9" t="s">
         <v>47</v>
       </c>
-      <c r="Q9" t="s">
+      <c r="R9" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>118</v>
       </c>
@@ -3641,46 +3652,46 @@
         <v>78</v>
       </c>
       <c r="D10" s="2"/>
-      <c r="P10" t="s">
+      <c r="Q10" t="s">
         <v>47</v>
       </c>
-      <c r="Q10" t="s">
+      <c r="R10" t="s">
         <v>77</v>
       </c>
-      <c r="R10" s="2"/>
-      <c r="S10" t="s">
+      <c r="S10" s="2"/>
+      <c r="T10" t="s">
         <v>187</v>
       </c>
-      <c r="T10" t="s">
+      <c r="U10" t="s">
         <v>186</v>
       </c>
-      <c r="U10" s="5" t="s">
+      <c r="V10" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="V10" s="5" t="s">
+      <c r="W10" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="W10" s="5"/>
-      <c r="Y10" s="5"/>
+      <c r="X10" s="5"/>
       <c r="Z10" s="5"/>
       <c r="AA10" s="5"/>
       <c r="AB10" s="5"/>
-    </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AC10" s="5"/>
+    </row>
+    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>119</v>
       </c>
-      <c r="AD11" s="5" t="s">
+      <c r="AE11" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="AE11" s="7" t="s">
+      <c r="AF11" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="AF11">
+      <c r="AG11">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>148</v>
       </c>
@@ -3691,12 +3702,12 @@
       <c r="E12" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="Q12" s="2"/>
       <c r="R12" s="2"/>
-      <c r="Y12" s="5"/>
+      <c r="S12" s="2"/>
       <c r="Z12" s="5"/>
-    </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AA12" s="5"/>
+    </row>
+    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>151</v>
       </c>
@@ -3719,37 +3730,38 @@
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
       <c r="O13" s="2"/>
-      <c r="Q13" s="10"/>
+      <c r="P13" s="2"/>
       <c r="R13" s="10"/>
-    </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="S13" s="10"/>
+    </row>
+    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>153</v>
       </c>
-      <c r="P14" t="s">
+      <c r="Q14" t="s">
         <v>48</v>
       </c>
-      <c r="Q14" t="s">
+      <c r="R14" t="s">
         <v>98</v>
       </c>
-      <c r="R14" t="s">
+      <c r="S14" t="s">
         <v>263</v>
       </c>
-      <c r="S14" t="s">
+      <c r="T14" t="s">
         <v>264</v>
       </c>
-      <c r="T14" t="s">
+      <c r="U14" t="s">
         <v>265</v>
       </c>
-      <c r="U14" s="5" t="s">
+      <c r="V14" s="5" t="s">
         <v>266</v>
       </c>
-      <c r="V14" s="5" t="s">
+      <c r="W14" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="W14" s="5"/>
-    </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="X14" s="5"/>
+    </row>
+    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>161</v>
       </c>
@@ -3775,33 +3787,34 @@
       <c r="M15" s="9"/>
       <c r="N15" s="9"/>
       <c r="O15" s="9"/>
-      <c r="P15" t="s">
+      <c r="P15" s="9"/>
+      <c r="Q15" t="s">
         <v>48</v>
       </c>
-      <c r="Q15" t="s">
+      <c r="R15" t="s">
         <v>98</v>
       </c>
-      <c r="R15" t="s">
+      <c r="S15" t="s">
         <v>162</v>
       </c>
-      <c r="S15" t="s">
+      <c r="T15" t="s">
         <v>163</v>
       </c>
-      <c r="T15" t="s">
+      <c r="U15" t="s">
         <v>164</v>
       </c>
-      <c r="U15" s="5" t="s">
+      <c r="V15" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="V15" s="5" t="s">
+      <c r="W15" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="W15" s="5"/>
-      <c r="Z15" s="5"/>
-      <c r="AB15" s="5"/>
-      <c r="AC15" s="7"/>
-    </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="X15" s="5"/>
+      <c r="AA15" s="5"/>
+      <c r="AC15" s="5"/>
+      <c r="AD15" s="7"/>
+    </row>
+    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>167</v>
       </c>
@@ -3827,128 +3840,132 @@
       <c r="M16" s="9"/>
       <c r="N16" s="9"/>
       <c r="O16" s="9"/>
-      <c r="P16" t="s">
+      <c r="P16" s="9"/>
+      <c r="Q16" t="s">
         <v>48</v>
       </c>
-      <c r="Q16" t="s">
+      <c r="R16" t="s">
         <v>98</v>
       </c>
-      <c r="R16" t="s">
+      <c r="S16" t="s">
         <v>169</v>
       </c>
-      <c r="S16" t="s">
+      <c r="T16" t="s">
         <v>170</v>
       </c>
-      <c r="T16" t="s">
+      <c r="U16" t="s">
         <v>171</v>
       </c>
-      <c r="U16" s="5" t="s">
+      <c r="V16" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="V16" s="5" t="s">
+      <c r="W16" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="W16" s="5"/>
       <c r="X16" s="5"/>
-    </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="Y16" s="5"/>
+    </row>
+    <row r="17" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>177</v>
       </c>
-      <c r="X17" t="s">
+      <c r="Y17" t="s">
         <v>256</v>
       </c>
-      <c r="Z17" s="5"/>
-      <c r="AB17" s="5" t="s">
+      <c r="AA17" s="5"/>
+      <c r="AC17" s="5" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>189</v>
       </c>
-      <c r="AC18" t="s">
+      <c r="AD18" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>198</v>
       </c>
-      <c r="M19" t="s">
+      <c r="N19" t="s">
         <v>224</v>
       </c>
-      <c r="P19" t="s">
+      <c r="Q19" t="s">
         <v>48</v>
       </c>
-      <c r="Q19" t="s">
+      <c r="R19" t="s">
         <v>98</v>
       </c>
-      <c r="AG19" t="s">
+      <c r="AH19" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>97</v>
       </c>
-      <c r="AB20" s="5" t="s">
+      <c r="AC20" s="5" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>217</v>
       </c>
       <c r="G21" t="s">
+        <v>290</v>
+      </c>
+      <c r="H21" t="s">
         <v>37</v>
       </c>
-      <c r="O21" t="s">
+      <c r="P21" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>219</v>
       </c>
-      <c r="L22" s="5" t="s">
+      <c r="M22" s="5" t="s">
         <v>289</v>
       </c>
-      <c r="M22" s="5" t="s">
+      <c r="N22" s="5" t="s">
         <v>221</v>
       </c>
-      <c r="N22" s="5" t="s">
+      <c r="O22" s="5" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>247</v>
       </c>
-      <c r="AH23" t="s">
+      <c r="AI23" t="s">
         <v>261</v>
       </c>
-      <c r="AI23" t="s">
+      <c r="AJ23" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="24" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>276</v>
       </c>
-      <c r="X24" t="s">
+      <c r="Y24" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="25" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>279</v>
       </c>
-      <c r="X25" t="s">
+      <c r="Y25" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="26" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>280</v>
       </c>
@@ -3956,73 +3973,73 @@
         <v>78</v>
       </c>
       <c r="D26" s="10"/>
-      <c r="L26" s="5" t="s">
+      <c r="M26" s="5" t="s">
         <v>289</v>
       </c>
-      <c r="M26" s="2"/>
       <c r="N26" s="2"/>
       <c r="O26" s="2"/>
-      <c r="P26" s="2" t="s">
+      <c r="P26" s="2"/>
+      <c r="Q26" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="Q26" t="s">
+      <c r="R26" t="s">
         <v>47</v>
       </c>
-      <c r="R26" t="s">
+      <c r="S26" t="s">
         <v>263</v>
       </c>
-      <c r="S26" t="s">
+      <c r="T26" t="s">
         <v>264</v>
       </c>
-      <c r="T26" t="s">
+      <c r="U26" t="s">
         <v>265</v>
       </c>
-      <c r="U26" s="5" t="s">
+      <c r="V26" s="5" t="s">
         <v>266</v>
       </c>
-      <c r="V26" s="5" t="s">
+      <c r="W26" s="5" t="s">
         <v>281</v>
       </c>
-      <c r="W26" s="5">
+      <c r="X26" s="5">
         <v>888888</v>
       </c>
-      <c r="X26" s="5"/>
-      <c r="Y26" s="24" t="s">
+      <c r="Y26" s="5"/>
+      <c r="Z26" s="24" t="s">
         <v>282</v>
       </c>
-      <c r="AA26" s="5"/>
       <c r="AB26" s="5"/>
       <c r="AC26" s="5"/>
-      <c r="AD26" s="5" t="s">
+      <c r="AD26" s="5"/>
+      <c r="AE26" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="AE26" s="5" t="s">
+      <c r="AF26" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="AF26" s="5">
+      <c r="AG26" s="5">
         <v>123</v>
       </c>
-      <c r="AG26" s="7"/>
-    </row>
-    <row r="27" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AH26" s="7"/>
+    </row>
+    <row r="27" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>122</v>
       </c>
-      <c r="H27" s="5" t="s">
+      <c r="I27" s="5" t="s">
         <v>283</v>
       </c>
-      <c r="I27" s="5" t="s">
+      <c r="J27" s="5" t="s">
         <v>284</v>
       </c>
-      <c r="J27" t="s">
+      <c r="K27" t="s">
         <v>47</v>
       </c>
-      <c r="K27" s="2" t="s">
+      <c r="L27" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="29" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="R29" s="5"/>
+    <row r="29" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="S29" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -4039,7 +4056,7 @@
     <hyperlink ref="C16" r:id="rId11" xr:uid="{50B14846-390B-41D6-AC9B-F1AB298F8D8C}"/>
     <hyperlink ref="C26" r:id="rId12" xr:uid="{5B11667E-8BEA-4F20-9718-31610EB2A4F7}"/>
     <hyperlink ref="D2" r:id="rId13" xr:uid="{27010551-28C9-440A-A2C5-A4B65C1CD387}"/>
-    <hyperlink ref="K27" r:id="rId14" xr:uid="{29605C66-2AFB-406F-A76E-289407A06171}"/>
+    <hyperlink ref="L27" r:id="rId14" xr:uid="{29605C66-2AFB-406F-A76E-289407A06171}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId15"/>

</xml_diff>

<commit_message>
87 testcase changes for the osprey emea
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Osprey_EMEA/GoldOspreyemeaEUFR.xlsx
+++ b/src/test/resources/TestData/Osprey_EMEA/GoldOspreyemeaEUFR.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BE65B4A-F633-4E36-8009-A074023230F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDBAACD7-6E69-45FC-95F1-56BC7D7BF2A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="10" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1045" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1047" uniqueCount="298">
   <si>
     <t>UserName</t>
   </si>
@@ -937,6 +937,18 @@
   </si>
   <si>
     <t>Mon Compte</t>
+  </si>
+  <si>
+    <t>Sacs à dos et sacs</t>
+  </si>
+  <si>
+    <t>Packs enfants et porte-bébés</t>
+  </si>
+  <si>
+    <t>Porte-bébés</t>
+  </si>
+  <si>
+    <t>Poco® Carrying Case</t>
   </si>
 </sst>
 </file>
@@ -1799,10 +1811,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB7898D0-5E73-467F-9FF3-820055A67CA5}">
-  <dimension ref="A1:X6"/>
+  <dimension ref="A1:Y6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1811,10 +1823,10 @@
     <col min="2" max="2" width="27.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="22" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="22" customWidth="1"/>
+    <col min="15" max="17" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1858,37 +1870,40 @@
         <v>15</v>
       </c>
       <c r="O1" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>52</v>
       </c>
@@ -1926,7 +1941,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>95</v>
       </c>
@@ -1936,50 +1951,53 @@
       <c r="N3" t="s">
         <v>257</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="R3" t="s">
         <v>278</v>
       </c>
-      <c r="R3" s="9" t="s">
+      <c r="S3" s="9" t="s">
         <v>204</v>
       </c>
-      <c r="S3" t="s">
-        <v>256</v>
-      </c>
-      <c r="T3" s="5" t="s">
+      <c r="T3" t="s">
+        <v>297</v>
+      </c>
+      <c r="U3" s="5" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>177</v>
       </c>
       <c r="N4" t="s">
-        <v>256</v>
-      </c>
-      <c r="T4" s="5" t="s">
+        <v>297</v>
+      </c>
+      <c r="U4" s="5" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>97</v>
       </c>
       <c r="C5" t="s">
         <v>289</v>
       </c>
-      <c r="T5" s="5" t="s">
+      <c r="U5" s="5" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>217</v>
       </c>
       <c r="O6" t="s">
-        <v>37</v>
+        <v>294</v>
       </c>
       <c r="P6" t="s">
-        <v>215</v>
+        <v>295</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>296</v>
       </c>
     </row>
   </sheetData>
@@ -3344,7 +3362,7 @@
   <dimension ref="A1:AJ29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4614,7 +4632,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A6E5005-1842-4D3B-9DB5-D7120C934727}">
   <dimension ref="A1:AJ9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>

</xml_diff>